<commit_message>
Make demo scripts TST962, TST966 and TST1172 point to the availabe devices.
</commit_message>
<xml_diff>
--- a/NformTester/NformTester/keywordscripts/TST1172_EditDeviceAlarmName.xlsx
+++ b/NformTester/NformTester/keywordscripts/TST1172_EditDeviceAlarmName.xlsx
@@ -1209,7 +1209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7576" uniqueCount="843">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7575" uniqueCount="843">
   <si>
     <t>FormLogin_to_LiebertR_Nform</t>
   </si>
@@ -3637,9 +3637,6 @@
     <t>;Clear operation.</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
     <t>;Create one device.</t>
   </si>
   <si>
@@ -3751,14 +3748,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>$SNMPdevice_0$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>$GXT_0_NAME$</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>"System Output Off"</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3772,6 +3761,18 @@
   </si>
   <si>
     <t>My System Output Off</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$SNMP_GXT_0_NAME$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>$SNMP_device_0$</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ClickItem</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -4704,8 +4705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H87" sqref="H87"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -4796,7 +4797,7 @@
         <v>768</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C3" s="5">
         <v>2</v>
@@ -4837,7 +4838,7 @@
         <v>3</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>18</v>
@@ -4868,7 +4869,7 @@
         <v>4</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
@@ -4903,22 +4904,22 @@
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5" t="s">
+        <v>822</v>
+      </c>
+      <c r="I6" s="5" t="s">
+        <v>841</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>840</v>
+      </c>
+      <c r="K6" s="5" t="s">
         <v>823</v>
       </c>
-      <c r="I6" s="5" t="s">
-        <v>837</v>
-      </c>
-      <c r="J6" s="5" t="s">
-        <v>838</v>
-      </c>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="5" t="s">
+        <v>830</v>
+      </c>
+      <c r="M6" s="5" t="s">
         <v>824</v>
-      </c>
-      <c r="L6" s="5" t="s">
-        <v>831</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>825</v>
       </c>
       <c r="N6" s="7"/>
       <c r="O6" s="2"/>
@@ -4934,7 +4935,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
@@ -4952,9 +4953,7 @@
       <c r="A8" s="3" t="s">
         <v>765</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>801</v>
-      </c>
+      <c r="B8" s="4"/>
       <c r="C8" s="5">
         <v>7</v>
       </c>
@@ -5026,10 +5025,10 @@
         <v>578</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>56</v>
+        <v>842</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -5144,10 +5143,10 @@
         <v>109</v>
       </c>
       <c r="G14" s="5" t="s">
+        <v>835</v>
+      </c>
+      <c r="H14" s="11" t="s">
         <v>836</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>839</v>
       </c>
       <c r="I14" s="11"/>
       <c r="J14" s="5"/>
@@ -5181,10 +5180,10 @@
         <v>799</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="J15" s="11" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
@@ -5216,10 +5215,10 @@
         <v>799</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="J16" s="11" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
@@ -5308,7 +5307,7 @@
         <v>4</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="I19" s="11"/>
       <c r="J19" s="5"/>
@@ -5356,7 +5355,7 @@
         <v>20</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="E21" s="11"/>
       <c r="F21" s="5"/>
@@ -5400,7 +5399,7 @@
         <v>22</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="E23" s="11"/>
       <c r="F23" s="5"/>
@@ -5481,7 +5480,7 @@
         <v>56</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="I26" s="11"/>
       <c r="J26" s="5"/>
@@ -5511,10 +5510,10 @@
         <v>799</v>
       </c>
       <c r="I27" s="5" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="J27" s="11" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
@@ -5542,10 +5541,10 @@
         <v>799</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="J28" s="11" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
@@ -5620,7 +5619,7 @@
         <v>4</v>
       </c>
       <c r="H31" s="11" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="I31" s="5"/>
       <c r="J31" s="5"/>
@@ -5710,7 +5709,7 @@
         <v>34</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="E35" s="11"/>
       <c r="F35" s="5"/>
@@ -5816,7 +5815,7 @@
         <v>56</v>
       </c>
       <c r="H39" s="11" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="I39" s="11"/>
       <c r="J39" s="5"/>
@@ -5846,10 +5845,10 @@
         <v>799</v>
       </c>
       <c r="I40" s="5" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="J40" s="11" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
@@ -5877,10 +5876,10 @@
         <v>799</v>
       </c>
       <c r="I41" s="5" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="J41" s="11" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
@@ -5968,7 +5967,7 @@
         <v>44</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="E45" s="11"/>
       <c r="F45" s="5"/>
@@ -5987,7 +5986,7 @@
         <v>45</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E46" s="5" t="s">
         <v>19</v>
@@ -6012,7 +6011,7 @@
         <v>46</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E47" s="5" t="s">
         <v>19</v>
@@ -6037,7 +6036,7 @@
         <v>47</v>
       </c>
       <c r="D48" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>306</v>
@@ -6049,10 +6048,10 @@
         <v>7</v>
       </c>
       <c r="H48" s="11" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="I48" s="5" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="J48" s="5" t="b">
         <v>1</v>
@@ -6091,7 +6090,7 @@
         <v>49</v>
       </c>
       <c r="D50" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E50" s="11" t="s">
         <v>306</v>
@@ -6116,7 +6115,7 @@
         <v>50</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E51" s="11" t="s">
         <v>310</v>
@@ -6128,7 +6127,7 @@
         <v>4</v>
       </c>
       <c r="H51" s="11" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
@@ -6143,7 +6142,7 @@
         <v>51</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E52" s="11" t="s">
         <v>310</v>
@@ -6155,7 +6154,7 @@
         <v>4</v>
       </c>
       <c r="H52" s="11" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
@@ -6170,7 +6169,7 @@
         <v>52</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E53" s="11" t="s">
         <v>310</v>
@@ -6245,7 +6244,7 @@
         <v>55</v>
       </c>
       <c r="D56" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E56" s="11" t="s">
         <v>361</v>
@@ -6257,7 +6256,7 @@
         <v>4</v>
       </c>
       <c r="H56" s="11" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="I56" s="11"/>
       <c r="J56" s="5"/>
@@ -6272,7 +6271,7 @@
         <v>56</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E57" s="11" t="s">
         <v>361</v>
@@ -6284,7 +6283,7 @@
         <v>4</v>
       </c>
       <c r="H57" s="11" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="I57" s="11"/>
       <c r="J57" s="5"/>
@@ -6311,7 +6310,7 @@
         <v>4</v>
       </c>
       <c r="H58" s="11" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="I58" s="11"/>
       <c r="J58" s="5"/>
@@ -6351,7 +6350,7 @@
         <v>59</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E60" s="11" t="s">
         <v>361</v>
@@ -6363,7 +6362,7 @@
         <v>4</v>
       </c>
       <c r="H60" s="11" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="I60" s="5"/>
       <c r="J60" s="5"/>
@@ -6378,7 +6377,7 @@
         <v>60</v>
       </c>
       <c r="D61" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E61" s="11" t="s">
         <v>361</v>
@@ -6390,7 +6389,7 @@
         <v>4</v>
       </c>
       <c r="H61" s="11" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="I61" s="5"/>
       <c r="J61" s="5"/>
@@ -6455,7 +6454,7 @@
         <v>63</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E64" s="11" t="s">
         <v>361</v>
@@ -6467,7 +6466,7 @@
         <v>13</v>
       </c>
       <c r="H64" s="11" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="I64" s="11"/>
       <c r="J64" s="5"/>
@@ -6494,7 +6493,7 @@
         <v>13</v>
       </c>
       <c r="H65" s="11" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="I65" s="5"/>
       <c r="J65" s="5"/>
@@ -6509,7 +6508,7 @@
         <v>65</v>
       </c>
       <c r="D66" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E66" s="11" t="s">
         <v>361</v>
@@ -6521,7 +6520,7 @@
         <v>13</v>
       </c>
       <c r="H66" s="11" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="I66" s="5"/>
       <c r="J66" s="5"/>
@@ -6536,7 +6535,7 @@
         <v>66</v>
       </c>
       <c r="D67" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E67" s="11" t="s">
         <v>361</v>
@@ -6548,7 +6547,7 @@
         <v>13</v>
       </c>
       <c r="H67" s="5" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="I67" s="5"/>
       <c r="J67" s="5"/>
@@ -6563,7 +6562,7 @@
         <v>67</v>
       </c>
       <c r="D68" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E68" s="11" t="s">
         <v>361</v>
@@ -6575,7 +6574,7 @@
         <v>13</v>
       </c>
       <c r="H68" s="11" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="I68" s="5"/>
       <c r="J68" s="5"/>
@@ -6590,7 +6589,7 @@
         <v>68</v>
       </c>
       <c r="D69" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E69" s="11" t="s">
         <v>361</v>
@@ -6617,7 +6616,7 @@
         <v>69</v>
       </c>
       <c r="D70" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E70" s="11" t="s">
         <v>361</v>
@@ -6642,7 +6641,7 @@
         <v>70</v>
       </c>
       <c r="D71" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E71" s="11" t="s">
         <v>361</v>
@@ -6667,7 +6666,7 @@
         <v>71</v>
       </c>
       <c r="D72" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E72" s="11" t="s">
         <v>361</v>
@@ -6754,7 +6753,7 @@
         <v>4</v>
       </c>
       <c r="H75" s="11" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="I75" s="11"/>
       <c r="J75" s="5"/>
@@ -6806,7 +6805,7 @@
         <v>59</v>
       </c>
       <c r="H77" s="11" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="I77" s="11"/>
       <c r="J77" s="5"/>
@@ -6869,7 +6868,7 @@
         <v>79</v>
       </c>
       <c r="D80" s="6" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="E80" s="11"/>
       <c r="F80" s="5"/>
@@ -6928,7 +6927,7 @@
         <v>2</v>
       </c>
       <c r="I82" s="5" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="J82" s="5"/>
       <c r="K82" s="5"/>
@@ -6954,7 +6953,7 @@
         <v>59</v>
       </c>
       <c r="H83" s="11" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="I83" s="11"/>
       <c r="J83" s="5"/>
@@ -7100,7 +7099,7 @@
         <v>56</v>
       </c>
       <c r="H89" s="5" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="I89" s="11"/>
       <c r="J89" s="5"/>
@@ -7190,7 +7189,7 @@
         <v>92</v>
       </c>
       <c r="D93" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E93" s="5" t="s">
         <v>19</v>
@@ -7215,7 +7214,7 @@
         <v>93</v>
       </c>
       <c r="D94" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E94" s="5" t="s">
         <v>19</v>
@@ -7240,7 +7239,7 @@
         <v>94</v>
       </c>
       <c r="D95" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E95" s="11" t="s">
         <v>306</v>
@@ -7252,7 +7251,7 @@
         <v>56</v>
       </c>
       <c r="H95" s="11" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="I95" s="5"/>
       <c r="J95" s="5"/>
@@ -7267,7 +7266,7 @@
         <v>95</v>
       </c>
       <c r="D96" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E96" s="11" t="s">
         <v>306</v>
@@ -7292,7 +7291,7 @@
         <v>96</v>
       </c>
       <c r="D97" s="8" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="E97" s="11" t="s">
         <v>306</v>
@@ -29312,22 +29311,22 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="B6" t="s">
         <v>391</v>
@@ -29339,7 +29338,7 @@
         <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
     </row>
   </sheetData>

</xml_diff>